<commit_message>
alteração cadastro sorteio e adicionado menu.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/doc/participantes.xlsx
+++ b/src/main/webapp/resources/doc/participantes.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sec03\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>NOME</t>
   </si>
@@ -36,13 +31,34 @@
   </si>
   <si>
     <t>TELEFONE</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
+    <t>14554648303</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>joao</t>
+  </si>
+  <si>
+    <t>13660191647</t>
+  </si>
+  <si>
+    <t>wesley</t>
+  </si>
+  <si>
+    <t>64218415200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,7 +233,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,21 +410,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="4" customWidth="1"/>
@@ -416,7 +432,7 @@
     <col min="4" max="4" width="13.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,6 +444,48 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>